<commit_message>
Data for gen collected :D
</commit_message>
<xml_diff>
--- a/scripts/valgrind_logs/data.xlsx
+++ b/scripts/valgrind_logs/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SchoolWork\FYP\Compiler Stuff\Code\graphiC\scripts\valgrind_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76AD014-9953-4D32-BAFE-7B132DADBF6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3226ED52-2DCC-497B-AB01-9638D3102282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-86" yWindow="0" windowWidth="11143" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>Generational</t>
   </si>
@@ -123,7 +123,25 @@
     <t>0.003403/0.000000</t>
   </si>
   <si>
-    <t>4-</t>
+    <t>4-write_barrier.txt</t>
+  </si>
+  <si>
+    <t>0.101839/0.000000</t>
+  </si>
+  <si>
+    <t>0.106112/0.000000</t>
+  </si>
+  <si>
+    <t>0.105315/0.000000</t>
+  </si>
+  <si>
+    <t>0.891102/0.000000</t>
+  </si>
+  <si>
+    <t>0.861264/0.000000</t>
+  </si>
+  <si>
+    <t>0.852867/0.000000</t>
   </si>
 </sst>
 </file>
@@ -168,13 +186,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -494,32 +512,32 @@
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1" t="s">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1" t="s">
+      <c r="F7" s="3"/>
+      <c r="G7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="1"/>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B8" s="2"/>
@@ -587,7 +605,7 @@
       <c r="H10" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -617,6 +635,24 @@
     <row r="12" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
         <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H12" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>